<commit_message>
Translated a column to english
</commit_message>
<xml_diff>
--- a/Tables for thesis resit 2021 - final.xlsx
+++ b/Tables for thesis resit 2021 - final.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miche\OneDrive\Documenten\Business Analytics and Management\Thesis\2. Thesis final\4. Analysis\Thesis BAM 2021\Thesis-BAM-Resit-2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B6C525F6-894F-4F7D-B7A9-EF70F3813510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{51E8B28F-06A8-424D-A5CE-5132C5B3F4DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="822" firstSheet="3" activeTab="8" xr2:uid="{32F80ADA-10F3-4B56-B6F6-E7140D6CDA28}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="822" xr2:uid="{32F80ADA-10F3-4B56-B6F6-E7140D6CDA28}"/>
   </bookViews>
   <sheets>
-    <sheet name="Opleidingen in de dataset" sheetId="1" r:id="rId1"/>
+    <sheet name="Educational Programmes" sheetId="1" r:id="rId1"/>
     <sheet name="Dependent variables" sheetId="2" r:id="rId2"/>
     <sheet name="RD &amp; KNN Results" sheetId="5" r:id="rId3"/>
     <sheet name="SV PF Papers" sheetId="6" r:id="rId4"/>
@@ -26,7 +26,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Comparing simulation results'!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'descriptive statistics categ.'!$A$35:$C$35</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Opleidingen in de dataset'!$E$2:$E$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Educational Programmes'!$E$2:$E$25</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'RD &amp; KNN Results'!$A$2:$D$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'SV PF Papers'!$B$70:$E$70</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Variables used per study '!$A$2:$E$2</definedName>
@@ -3631,8 +3631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AB975B9-1822-4F87-BED2-7204DACE8E6A}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -74481,7 +74481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E930D319-DF08-4AA0-B8D8-42B0B52D1CFB}">
   <dimension ref="C11:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>

</xml_diff>